<commit_message>
[Memoria] Pruebas y Profiling
Añadidas sección de profiling en Pruebas. Explicados experimentos SOM.
</commit_message>
<xml_diff>
--- a/memoria/tablasygraficas.xlsx
+++ b/memoria/tablasygraficas.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xKuZz\Desktop\TFG1819\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\tfg\memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9467774D-42A6-4FDB-94BD-23616BD55376}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ÁRBOL" sheetId="2" r:id="rId1"/>
     <sheet name="SUSY-RF" sheetId="1" r:id="rId2"/>
     <sheet name="SUSY-SOM" sheetId="3" r:id="rId3"/>
+    <sheet name="Profiler SOM" sheetId="4" r:id="rId4"/>
+    <sheet name="Profiler Árbol" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'SUSY-RF'!$A$3</definedName>
@@ -26,17 +29,22 @@
     <definedName name="_xlchart.v1.6" hidden="1">'SUSY-RF'!$H$3</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'SUSY-RF'!$H$4:$H$13</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>CUDA</t>
   </si>
@@ -208,11 +216,50 @@
   <si>
     <t>GANANCIA</t>
   </si>
+  <si>
+    <t>Cálculo pesos parciales</t>
+  </si>
+  <si>
+    <t>Cálculo de distancia euclídea</t>
+  </si>
+  <si>
+    <t>Datos [Host -&gt; Dispositivo]</t>
+  </si>
+  <si>
+    <t>Encontrar mejor BMU (Reducción)</t>
+  </si>
+  <si>
+    <t>Datos [Dispositivo -&gt; Host]</t>
+  </si>
+  <si>
+    <t>Actividad GPU</t>
+  </si>
+  <si>
+    <t>Porcentaje de tiempo (%)</t>
+  </si>
+  <si>
+    <t>Scan</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Reorganizar listas de atributos</t>
+  </si>
+  <si>
+    <t>Ordenar listas de atributos [Inicio]</t>
+  </si>
+  <si>
+    <t>Podar nodo [Reducción suma]</t>
+  </si>
+  <si>
+    <t>Encontrar mejor punto de corte [Cálculo del criterio y reducción]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -242,12 +289,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4331,7 +4381,7 @@
                   <c:v>1172.1199999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1191</c:v>
+                  <c:v>1205.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4471,7 +4521,7 @@
                   <c:v>1181.462</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1205.79</c:v>
+                  <c:v>1197.5920000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4610,7 +4660,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4708,22 +4757,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -4733,7 +4776,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4747,22 +4789,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="es-ES"/>
@@ -4791,42 +4827,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
@@ -4882,7 +4889,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="300"/>
+        <c:gapWidth val="247"/>
         <c:axId val="407073567"/>
         <c:axId val="407067327"/>
       </c:barChart>
@@ -4904,63 +4911,28 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="6"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
@@ -5063,63 +5035,28 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="6"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent2">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent2">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
@@ -5195,7 +5132,7 @@
                   <c:v>1181.462</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1205.79</c:v>
+                  <c:v>1197.5920000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5219,7 +5156,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -5238,17 +5178,31 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -5260,10 +5214,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -5292,9 +5247,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -5320,8 +5275,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -5361,8 +5317,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -5384,7 +5341,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="407067327"/>
@@ -5401,13 +5358,14 @@
         <c:showKeys val="1"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -5416,13 +5374,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr rtl="0">
-              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -5435,7 +5391,17 @@
         </c:txPr>
       </c:dTable>
       <c:spPr>
-        <a:noFill/>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -5444,7 +5410,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5460,8 +5425,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -5478,28 +5444,1036 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Tiempo de ejecución de</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> las actividades de la GPU en el mapa autoorganizado</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent2">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="accent2">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent2">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Profiler SOM'!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje de tiempo (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Profiler SOM'!$A$6:$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Cálculo pesos parciales</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cálculo de distancia euclídea</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Datos [Host -&gt; Dispositivo]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Encontrar mejor BMU (Reducción)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Datos [Dispositivo -&gt; Host]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Profiler SOM'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.58630000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5600000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7099999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EEB4-40E5-9C59-7417E1E8D8E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
           </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1"/>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="10000"/>
+          <a:lumOff val="90000"/>
+        </a:schemeClr>
+      </a:bgClr>
+    </a:pattFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Tiempo de ejecución de</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> las actividades de la GPU en el árbol de decisión</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent2">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="accent2">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent2">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B699-4791-91F0-41BD0EF83472}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B699-4791-91F0-41BD0EF83472}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B699-4791-91F0-41BD0EF83472}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-B699-4791-91F0-41BD0EF83472}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-B699-4791-91F0-41BD0EF83472}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Profiler Árbol'!$A$1:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Scan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ordenar listas de atributos [Inicio]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Datos [Dispositivo -&gt; Host]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Datos [Host -&gt; Dispositivo]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Reorganizar listas de atributos</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Encontrar mejor punto de corte [Cálculo del criterio y reducción]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Podar nodo [Reducción suma]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Profiler Árbol'!$B$1:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>46.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.070000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-B699-4791-91F0-41BD0EF83472}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
           </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1"/>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="10000"/>
+          <a:lumOff val="90000"/>
+        </a:schemeClr>
+      </a:bgClr>
+    </a:pattFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -5847,6 +6821,83 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9095,83 +10146,8 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="328">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="221">
   <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -9181,10 +10157,88 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -9193,35 +10247,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -9233,15 +10297,18 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -9254,10 +10321,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -9273,56 +10340,46 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="95000"/>
-              <a:lumOff val="5000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="75000"/>
-              <a:lumOff val="25000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-      </a:gradFill>
-      <a:ln w="9525">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -9331,12 +10388,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -9347,13 +10407,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9365,22 +10426,35 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9392,16 +10466,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -9410,12 +10485,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -9426,16 +10504,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -9444,8 +10523,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -9455,37 +10535,45 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
   </cs:plotArea>
   <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:plotArea3D>
   <cs:seriesAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -9493,14 +10581,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9511,20 +10599,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -9533,7 +10614,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -9548,8 +10629,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -9559,27 +10641,574 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="256">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="10000"/>
+            <a:lumOff val="90000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:gradFill>
         <a:gsLst>
           <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="85000"/>
+            <a:schemeClr val="phClr">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
             </a:schemeClr>
           </a:gs>
           <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="phClr"/>
           </a:gs>
         </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
+        <a:lin ang="5400000" scaled="0"/>
       </a:gradFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:ln w="50800">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -9590,8 +11219,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -9601,7 +11231,550 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="256">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="10000"/>
+            <a:lumOff val="90000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:ln w="50800">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -9624,7 +11797,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -9654,7 +11833,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -9686,7 +11871,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -9716,7 +11907,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Gráfico 7"/>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -9755,7 +11952,13 @@
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Gráfico 1"/>
+            <xdr:cNvPr id="2" name="Gráfico 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -9778,6 +11981,10 @@
             </xdr:cNvSpPr>
           </xdr:nvSpPr>
           <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2600325" y="3267075"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -9826,7 +12033,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Gráfico 7"/>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -9856,8 +12069,198 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Gráfico 9"/>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FBF7479-7F31-4433-BB7B-6CB62DC83503}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>652096</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>131884</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>592015</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>54582</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66406162-BD59-413B-A844-6BCFB4821176}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="652096" y="5084884"/>
+          <a:ext cx="10058400" cy="2780198"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>100777</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48234FAA-43AB-44FD-8412-7432BBB96AD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7153275"/>
+          <a:ext cx="10058400" cy="5330002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3829AACA-C740-4C88-99B8-AD2E5928FF49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -10136,7 +12539,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L12"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -10491,7 +12894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10894,11 +13297,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11330,7 +13733,7 @@
         <v>1172.1199999999999</v>
       </c>
       <c r="K13">
-        <v>1191</v>
+        <v>1205.79</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -11342,7 +13745,7 @@
         <v>1024.6820000000002</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:K14" si="1">SUM(C9:C13)/5</f>
+        <f t="shared" ref="C14:J14" si="1">SUM(C9:C13)/5</f>
         <v>1038.77</v>
       </c>
       <c r="D14">
@@ -11374,7 +13777,8 @@
         <v>1181.462</v>
       </c>
       <c r="K14">
-        <v>1205.79</v>
+        <f>SUM(K9:K13)/5</f>
+        <v>1197.5920000000001</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -11418,7 +13822,7 @@
         <v>7.2171597563019372</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="2"/>
+        <f>K8/K13</f>
         <v>7.8012058484479061</v>
       </c>
     </row>
@@ -11793,10 +14197,269 @@
         <f>K7</f>
         <v>9397.33</v>
       </c>
-      <c r="U23">
-        <f>K13</f>
-        <v>1191</v>
-      </c>
+      <c r="U23" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128B6458-FFCD-4BBA-89F2-3032037E7737}">
+  <dimension ref="A5:B10"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.58630000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.32100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6.5600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2.7099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C241B48C-363D-49DC-B9A0-F3FCA400F26C}">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.28515625" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1">
+        <f>SUM(C1:F1)</f>
+        <v>46.27</v>
+      </c>
+      <c r="C1">
+        <v>15.17</v>
+      </c>
+      <c r="D1">
+        <v>12.25</v>
+      </c>
+      <c r="E1">
+        <v>12.07</v>
+      </c>
+      <c r="F1">
+        <v>6.78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2">
+        <f>SUM(C2:L2)</f>
+        <v>22.27</v>
+      </c>
+      <c r="C2">
+        <v>5.81</v>
+      </c>
+      <c r="D2">
+        <v>4.8</v>
+      </c>
+      <c r="E2">
+        <v>4.42</v>
+      </c>
+      <c r="F2">
+        <v>2.95</v>
+      </c>
+      <c r="G2">
+        <v>2.8</v>
+      </c>
+      <c r="H2">
+        <v>0.47</v>
+      </c>
+      <c r="I2">
+        <v>0.38</v>
+      </c>
+      <c r="J2">
+        <v>0.2</v>
+      </c>
+      <c r="K2">
+        <v>0.17</v>
+      </c>
+      <c r="L2">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>5.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <f>SUM(C5:I5)</f>
+        <v>14.070000000000002</v>
+      </c>
+      <c r="C5">
+        <v>3.46</v>
+      </c>
+      <c r="D5">
+        <v>3.12</v>
+      </c>
+      <c r="E5">
+        <v>3.9</v>
+      </c>
+      <c r="F5">
+        <v>2.06</v>
+      </c>
+      <c r="G5">
+        <v>0.91</v>
+      </c>
+      <c r="H5">
+        <v>0.54</v>
+      </c>
+      <c r="I5">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6">
+        <f>SUM(C6:F6)</f>
+        <v>5.32</v>
+      </c>
+      <c r="C6">
+        <v>0.62</v>
+      </c>
+      <c r="D6">
+        <v>3.07</v>
+      </c>
+      <c r="E6">
+        <v>0.59</v>
+      </c>
+      <c r="F6">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7">
+        <f>SUM(C7:D7)</f>
+        <v>0.51</v>
+      </c>
+      <c r="C7">
+        <v>0.38</v>
+      </c>
+      <c r="D7">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B1:B7)</f>
+        <v>100.02000000000002</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambios y pruebas nuevas.
</commit_message>
<xml_diff>
--- a/memoria/tablasygraficas.xlsx
+++ b/memoria/tablasygraficas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\tfg\memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9467774D-42A6-4FDB-94BD-23616BD55376}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7234A89D-7919-4C9C-A107-879DBBE8071B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17925" yWindow="3390" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ÁRBOL" sheetId="2" r:id="rId1"/>
@@ -292,12 +292,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2968,36 +2968,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1626.72</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2479.12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3329.27</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4196.71</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5061.9399999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5952.79</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6787.29</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7692.16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8527.35</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9413.42</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3106,34 +3076,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1604.72</c:v>
+                  <c:v>230.31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2470.77</c:v>
+                  <c:v>428.47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3335.34</c:v>
+                  <c:v>611.04</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4194.3100000000004</c:v>
+                  <c:v>822</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5089.2299999999996</c:v>
+                  <c:v>1001.56</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5943.89</c:v>
+                  <c:v>1192.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6789.89</c:v>
+                  <c:v>1396.48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7693.64</c:v>
+                  <c:v>1636.69</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8515.6200000000008</c:v>
+                  <c:v>1782.32</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9413.25</c:v>
+                  <c:v>1990.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3243,34 +3213,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1604.08</c:v>
+                  <c:v>230.93</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2472.04</c:v>
+                  <c:v>424.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3333.09</c:v>
+                  <c:v>629.54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4189.8999999999996</c:v>
+                  <c:v>825.71</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5080.2700000000004</c:v>
+                  <c:v>1012.31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5932.37</c:v>
+                  <c:v>1215.03</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6800.49</c:v>
+                  <c:v>1391.76</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7677.75</c:v>
+                  <c:v>1606.99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8520.68</c:v>
+                  <c:v>1783</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9402.94</c:v>
+                  <c:v>1986.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3380,34 +3350,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1600.76</c:v>
+                  <c:v>230.84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2472.91</c:v>
+                  <c:v>425.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3326.2</c:v>
+                  <c:v>610.73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4184.97</c:v>
+                  <c:v>819.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5080.3100000000004</c:v>
+                  <c:v>1029.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5536.83</c:v>
+                  <c:v>1237.9000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6824.09</c:v>
+                  <c:v>1410.11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7683.1</c:v>
+                  <c:v>1609.66</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8542.1200000000008</c:v>
+                  <c:v>1800.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9406.14</c:v>
+                  <c:v>1988.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3517,34 +3487,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1600.32</c:v>
+                  <c:v>232.28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2473.7800000000002</c:v>
+                  <c:v>426.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3328.62</c:v>
+                  <c:v>621.86</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4189.03</c:v>
+                  <c:v>823.22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5071.04</c:v>
+                  <c:v>1026.18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5934.39</c:v>
+                  <c:v>1203.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6832.6</c:v>
+                  <c:v>1394.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7674.61</c:v>
+                  <c:v>1613.38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8528.23</c:v>
+                  <c:v>1787.79</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9397.33</c:v>
+                  <c:v>2005.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3651,37 +3621,37 @@
             <c:numRef>
               <c:f>'SUSY-SOM'!$B$8:$K$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1607.3200000000002</c:v>
+                  <c:v>231.09</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2473.7240000000002</c:v>
+                  <c:v>426.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3330.5039999999999</c:v>
+                  <c:v>618.29250000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4190.9839999999995</c:v>
+                  <c:v>822.54500000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5076.558</c:v>
+                  <c:v>1017.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5860.0539999999992</c:v>
+                  <c:v>1212.1174999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6806.8720000000003</c:v>
+                  <c:v>1398.0924999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7684.2520000000004</c:v>
+                  <c:v>1616.68</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8526.7999999999993</c:v>
+                  <c:v>1788.5024999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9406.616</c:v>
+                  <c:v>1992.6100000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3793,36 +3763,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1040.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1038.19</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1069.3599999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1096.42</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1114.92</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1142.01</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1156.56</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1170.1600000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1174.6500000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1195.82</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3934,34 +3874,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1014.21</c:v>
+                  <c:v>56.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1039.67</c:v>
+                  <c:v>58.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1067.6400000000001</c:v>
+                  <c:v>59.23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1083.48</c:v>
+                  <c:v>67.319999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1124.8599999999999</c:v>
+                  <c:v>68.709999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1142.4100000000001</c:v>
+                  <c:v>63.13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1157.97</c:v>
+                  <c:v>64.89</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1177.8699999999999</c:v>
+                  <c:v>72.31</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1182.8399999999999</c:v>
+                  <c:v>73.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1191.4000000000001</c:v>
+                  <c:v>68.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4074,34 +4014,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1017.07</c:v>
+                  <c:v>56.65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1036.08</c:v>
+                  <c:v>59.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1065.1500000000001</c:v>
+                  <c:v>59.44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1093.49</c:v>
+                  <c:v>60.96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1119.49</c:v>
+                  <c:v>62.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1132.17</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1151.24</c:v>
+                  <c:v>67.31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1173.32</c:v>
+                  <c:v>65.94</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1179.25</c:v>
+                  <c:v>67.209999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1191.75</c:v>
+                  <c:v>73.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4214,34 +4154,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1025.28</c:v>
+                  <c:v>57.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1037.67</c:v>
+                  <c:v>58.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1065.5999999999999</c:v>
+                  <c:v>59.67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1095.9100000000001</c:v>
+                  <c:v>61.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1118.79</c:v>
+                  <c:v>62.14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1137.17</c:v>
+                  <c:v>71.56</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1158.17</c:v>
+                  <c:v>71.77</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1162.43</c:v>
+                  <c:v>66.180000000000007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1198.45</c:v>
+                  <c:v>66.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1203.2</c:v>
+                  <c:v>73.599999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4354,34 +4294,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1026.55</c:v>
+                  <c:v>56.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1042.24</c:v>
+                  <c:v>58.68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1072.69</c:v>
+                  <c:v>67.28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1094.21</c:v>
+                  <c:v>61.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1120.6500000000001</c:v>
+                  <c:v>71.81</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1134.6199999999999</c:v>
+                  <c:v>65.290000000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1168.98</c:v>
+                  <c:v>64.569999999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1175.56</c:v>
+                  <c:v>66.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1172.1199999999999</c:v>
+                  <c:v>66.73</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1205.79</c:v>
+                  <c:v>73.819999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4491,37 +4431,37 @@
             <c:numRef>
               <c:f>'SUSY-SOM'!$B$14:$K$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1024.6820000000002</c:v>
+                  <c:v>56.987500000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1038.77</c:v>
+                  <c:v>58.735000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1068.0880000000002</c:v>
+                  <c:v>61.404999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1092.702</c:v>
+                  <c:v>62.730000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1119.7419999999997</c:v>
+                  <c:v>66.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1137.6759999999999</c:v>
+                  <c:v>67.745000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1158.5840000000001</c:v>
+                  <c:v>67.134999999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1171.8679999999999</c:v>
+                  <c:v>67.632499999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1181.462</c:v>
+                  <c:v>68.452500000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1197.5920000000001</c:v>
+                  <c:v>72.294999999999987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4843,34 +4783,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.5686037229111078</c:v>
+                  <c:v>4.0550998025882867</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3813972294155592</c:v>
+                  <c:v>7.2561079424533919</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1181925084824464</c:v>
+                  <c:v>10.069090464945853</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.835431801168113</c:v>
+                  <c:v>13.112466124661246</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5336854382527418</c:v>
+                  <c:v>15.364693446088795</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1508988499361852</c:v>
+                  <c:v>17.892353679238315</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.8751648564109296</c:v>
+                  <c:v>20.825091234080581</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5572675420781188</c:v>
+                  <c:v>23.90389235944258</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.2171597563019372</c:v>
+                  <c:v>26.127643256272595</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.8012058484479061</c:v>
+                  <c:v>26.99282037388242</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4978,37 +4918,37 @@
             <c:numRef>
               <c:f>'SUSY-SOM'!$B$8:$K$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1607.3200000000002</c:v>
+                  <c:v>231.09</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2473.7240000000002</c:v>
+                  <c:v>426.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3330.5039999999999</c:v>
+                  <c:v>618.29250000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4190.9839999999995</c:v>
+                  <c:v>822.54500000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5076.558</c:v>
+                  <c:v>1017.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5860.0539999999992</c:v>
+                  <c:v>1212.1174999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6806.8720000000003</c:v>
+                  <c:v>1398.0924999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7684.2520000000004</c:v>
+                  <c:v>1616.68</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8526.7999999999993</c:v>
+                  <c:v>1788.5024999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9406.616</c:v>
+                  <c:v>1992.6100000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5102,37 +5042,37 @@
             <c:numRef>
               <c:f>'SUSY-SOM'!$B$14:$K$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1024.6820000000002</c:v>
+                  <c:v>56.987500000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1038.77</c:v>
+                  <c:v>58.735000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1068.0880000000002</c:v>
+                  <c:v>61.404999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1092.702</c:v>
+                  <c:v>62.730000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1119.7419999999997</c:v>
+                  <c:v>66.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1137.6759999999999</c:v>
+                  <c:v>67.745000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1158.5840000000001</c:v>
+                  <c:v>67.134999999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1171.8679999999999</c:v>
+                  <c:v>67.632499999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1181.462</c:v>
+                  <c:v>68.452500000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1197.5920000000001</c:v>
+                  <c:v>72.294999999999987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5257,7 +5197,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5633,6 +5573,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-2320-4BF9-BCD7-7CDE59713939}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -5659,6 +5604,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2320-4BF9-BCD7-7CDE59713939}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -5685,6 +5635,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-2320-4BF9-BCD7-7CDE59713939}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -5711,6 +5666,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-2320-4BF9-BCD7-7CDE59713939}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -5737,6 +5697,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-2320-4BF9-BCD7-7CDE59713939}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -6246,6 +6211,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-008D-492F-B406-54CD11B96DF5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -6275,6 +6245,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-008D-492F-B406-54CD11B96DF5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -12552,39 +12527,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="5"/>
       <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -12897,8 +12872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12910,36 +12885,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -13300,8 +13275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:U23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13345,70 +13320,40 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
-        <v>1626.72</v>
-      </c>
-      <c r="C3">
-        <v>2479.12</v>
-      </c>
-      <c r="D3">
-        <v>3329.27</v>
-      </c>
-      <c r="E3">
-        <v>4196.71</v>
-      </c>
-      <c r="F3">
-        <v>5061.9399999999996</v>
-      </c>
-      <c r="G3">
-        <v>5952.79</v>
-      </c>
-      <c r="H3">
-        <v>6787.29</v>
-      </c>
-      <c r="I3">
-        <v>7692.16</v>
-      </c>
-      <c r="J3">
-        <v>8527.35</v>
-      </c>
-      <c r="K3">
-        <v>9413.42</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4">
-        <v>1604.72</v>
+        <v>230.31</v>
       </c>
       <c r="C4">
-        <v>2470.77</v>
+        <v>428.47</v>
       </c>
       <c r="D4">
-        <v>3335.34</v>
+        <v>611.04</v>
       </c>
       <c r="E4">
-        <v>4194.3100000000004</v>
+        <v>822</v>
       </c>
       <c r="F4">
-        <v>5089.2299999999996</v>
+        <v>1001.56</v>
       </c>
       <c r="G4">
-        <v>5943.89</v>
+        <v>1192.5</v>
       </c>
       <c r="H4">
-        <v>6789.89</v>
+        <v>1396.48</v>
       </c>
       <c r="I4">
-        <v>7693.64</v>
+        <v>1636.69</v>
       </c>
       <c r="J4">
-        <v>8515.6200000000008</v>
+        <v>1782.32</v>
       </c>
       <c r="K4">
-        <v>9413.25</v>
+        <v>1990.52</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -13416,34 +13361,34 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>1604.08</v>
+        <v>230.93</v>
       </c>
       <c r="C5">
-        <v>2472.04</v>
+        <v>424.01</v>
       </c>
       <c r="D5">
-        <v>3333.09</v>
+        <v>629.54</v>
       </c>
       <c r="E5">
-        <v>4189.8999999999996</v>
+        <v>825.71</v>
       </c>
       <c r="F5">
-        <v>5080.2700000000004</v>
+        <v>1012.31</v>
       </c>
       <c r="G5">
-        <v>5932.37</v>
+        <v>1215.03</v>
       </c>
       <c r="H5">
-        <v>6800.49</v>
+        <v>1391.76</v>
       </c>
       <c r="I5">
-        <v>7677.75</v>
+        <v>1606.99</v>
       </c>
       <c r="J5">
-        <v>8520.68</v>
+        <v>1783</v>
       </c>
       <c r="K5">
-        <v>9402.94</v>
+        <v>1986.35</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -13451,34 +13396,34 @@
         <v>27</v>
       </c>
       <c r="B6">
-        <v>1600.76</v>
+        <v>230.84</v>
       </c>
       <c r="C6">
-        <v>2472.91</v>
+        <v>425.76</v>
       </c>
       <c r="D6">
-        <v>3326.2</v>
+        <v>610.73</v>
       </c>
       <c r="E6">
-        <v>4184.97</v>
+        <v>819.25</v>
       </c>
       <c r="F6">
-        <v>5080.3100000000004</v>
+        <v>1029.75</v>
       </c>
       <c r="G6">
-        <v>5536.83</v>
+        <v>1237.9000000000001</v>
       </c>
       <c r="H6">
-        <v>6824.09</v>
+        <v>1410.11</v>
       </c>
       <c r="I6">
-        <v>7683.1</v>
+        <v>1609.66</v>
       </c>
       <c r="J6">
-        <v>8542.1200000000008</v>
+        <v>1800.9</v>
       </c>
       <c r="K6">
-        <v>9406.14</v>
+        <v>1988.15</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -13486,149 +13431,119 @@
         <v>28</v>
       </c>
       <c r="B7">
-        <v>1600.32</v>
+        <v>232.28</v>
       </c>
       <c r="C7">
-        <v>2473.7800000000002</v>
+        <v>426.51</v>
       </c>
       <c r="D7">
-        <v>3328.62</v>
+        <v>621.86</v>
       </c>
       <c r="E7">
-        <v>4189.03</v>
+        <v>823.22</v>
       </c>
       <c r="F7">
-        <v>5071.04</v>
+        <v>1026.18</v>
       </c>
       <c r="G7">
-        <v>5934.39</v>
+        <v>1203.04</v>
       </c>
       <c r="H7">
-        <v>6832.6</v>
+        <v>1394.02</v>
       </c>
       <c r="I7">
-        <v>7674.61</v>
+        <v>1613.38</v>
       </c>
       <c r="J7">
-        <v>8528.23</v>
+        <v>1787.79</v>
       </c>
       <c r="K7">
-        <v>9397.33</v>
+        <v>2005.42</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B8">
-        <f>SUM(B3:B7)/5</f>
-        <v>1607.3200000000002</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ref="C8:K8" si="0">SUM(C3:C7)/5</f>
-        <v>2473.7240000000002</v>
-      </c>
-      <c r="D8">
+      <c r="B8" s="1">
+        <f>SUM(B4:B7)/4</f>
+        <v>231.09</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:K8" si="0">SUM(C4:C7)/4</f>
+        <v>426.1875</v>
+      </c>
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>3330.5039999999999</v>
-      </c>
-      <c r="E8">
+        <v>618.29250000000002</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>4190.9839999999995</v>
-      </c>
-      <c r="F8">
+        <v>822.54500000000007</v>
+      </c>
+      <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>5076.558</v>
-      </c>
-      <c r="G8">
+        <v>1017.45</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>5860.0539999999992</v>
-      </c>
-      <c r="H8">
+        <v>1212.1174999999998</v>
+      </c>
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
-        <v>6806.8720000000003</v>
-      </c>
-      <c r="I8">
+        <v>1398.0924999999997</v>
+      </c>
+      <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>7684.2520000000004</v>
-      </c>
-      <c r="J8">
+        <v>1616.68</v>
+      </c>
+      <c r="J8" s="1">
         <f t="shared" si="0"/>
-        <v>8526.7999999999993</v>
-      </c>
-      <c r="K8">
+        <v>1788.5024999999998</v>
+      </c>
+      <c r="K8" s="1">
         <f t="shared" si="0"/>
-        <v>9406.616</v>
+        <v>1992.6100000000001</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9">
-        <v>1040.3</v>
-      </c>
-      <c r="C9">
-        <v>1038.19</v>
-      </c>
-      <c r="D9">
-        <v>1069.3599999999999</v>
-      </c>
-      <c r="E9">
-        <v>1096.42</v>
-      </c>
-      <c r="F9">
-        <v>1114.92</v>
-      </c>
-      <c r="G9">
-        <v>1142.01</v>
-      </c>
-      <c r="H9">
-        <v>1156.56</v>
-      </c>
-      <c r="I9">
-        <v>1170.1600000000001</v>
-      </c>
-      <c r="J9">
-        <v>1174.6500000000001</v>
-      </c>
-      <c r="K9">
-        <v>1195.82</v>
-      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
       <c r="B10">
-        <v>1014.21</v>
+        <v>56.82</v>
       </c>
       <c r="C10">
-        <v>1039.67</v>
+        <v>58.25</v>
       </c>
       <c r="D10">
-        <v>1067.6400000000001</v>
+        <v>59.23</v>
       </c>
       <c r="E10">
-        <v>1083.48</v>
+        <v>67.319999999999993</v>
       </c>
       <c r="F10">
-        <v>1124.8599999999999</v>
+        <v>68.709999999999994</v>
       </c>
       <c r="G10">
-        <v>1142.4100000000001</v>
+        <v>63.13</v>
       </c>
       <c r="H10">
-        <v>1157.97</v>
+        <v>64.89</v>
       </c>
       <c r="I10">
-        <v>1177.8699999999999</v>
+        <v>72.31</v>
       </c>
       <c r="J10">
-        <v>1182.8399999999999</v>
+        <v>73.08</v>
       </c>
       <c r="K10">
-        <v>1191.4000000000001</v>
+        <v>68.2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -13636,34 +13551,34 @@
         <v>32</v>
       </c>
       <c r="B11">
-        <v>1017.07</v>
+        <v>56.65</v>
       </c>
       <c r="C11">
-        <v>1036.08</v>
+        <v>59.24</v>
       </c>
       <c r="D11">
-        <v>1065.1500000000001</v>
+        <v>59.44</v>
       </c>
       <c r="E11">
-        <v>1093.49</v>
+        <v>60.96</v>
       </c>
       <c r="F11">
-        <v>1119.49</v>
+        <v>62.22</v>
       </c>
       <c r="G11">
-        <v>1132.17</v>
+        <v>71</v>
       </c>
       <c r="H11">
-        <v>1151.24</v>
+        <v>67.31</v>
       </c>
       <c r="I11">
-        <v>1173.32</v>
+        <v>65.94</v>
       </c>
       <c r="J11">
-        <v>1179.25</v>
+        <v>67.209999999999994</v>
       </c>
       <c r="K11">
-        <v>1191.75</v>
+        <v>73.56</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -13671,34 +13586,34 @@
         <v>33</v>
       </c>
       <c r="B12">
-        <v>1025.28</v>
+        <v>57.7</v>
       </c>
       <c r="C12">
-        <v>1037.67</v>
+        <v>58.77</v>
       </c>
       <c r="D12">
-        <v>1065.5999999999999</v>
+        <v>59.67</v>
       </c>
       <c r="E12">
-        <v>1095.9100000000001</v>
+        <v>61.24</v>
       </c>
       <c r="F12">
-        <v>1118.79</v>
+        <v>62.14</v>
       </c>
       <c r="G12">
-        <v>1137.17</v>
+        <v>71.56</v>
       </c>
       <c r="H12">
-        <v>1158.17</v>
+        <v>71.77</v>
       </c>
       <c r="I12">
-        <v>1162.43</v>
+        <v>66.180000000000007</v>
       </c>
       <c r="J12">
-        <v>1198.45</v>
+        <v>66.790000000000006</v>
       </c>
       <c r="K12">
-        <v>1203.2</v>
+        <v>73.599999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -13706,79 +13621,79 @@
         <v>34</v>
       </c>
       <c r="B13">
-        <v>1026.55</v>
+        <v>56.78</v>
       </c>
       <c r="C13">
-        <v>1042.24</v>
+        <v>58.68</v>
       </c>
       <c r="D13">
-        <v>1072.69</v>
+        <v>67.28</v>
       </c>
       <c r="E13">
-        <v>1094.21</v>
+        <v>61.4</v>
       </c>
       <c r="F13">
-        <v>1120.6500000000001</v>
+        <v>71.81</v>
       </c>
       <c r="G13">
-        <v>1134.6199999999999</v>
+        <v>65.290000000000006</v>
       </c>
       <c r="H13">
-        <v>1168.98</v>
+        <v>64.569999999999993</v>
       </c>
       <c r="I13">
-        <v>1175.56</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="J13">
-        <v>1172.1199999999999</v>
+        <v>66.73</v>
       </c>
       <c r="K13">
-        <v>1205.79</v>
+        <v>73.819999999999993</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B14">
-        <f>SUM(B9:B13)/5</f>
-        <v>1024.6820000000002</v>
-      </c>
-      <c r="C14">
-        <f t="shared" ref="C14:J14" si="1">SUM(C9:C13)/5</f>
-        <v>1038.77</v>
-      </c>
-      <c r="D14">
+      <c r="B14" s="1">
+        <f>SUM(B10:B13)/4</f>
+        <v>56.987500000000004</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:K14" si="1">SUM(C10:C13)/4</f>
+        <v>58.735000000000007</v>
+      </c>
+      <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>1068.0880000000002</v>
-      </c>
-      <c r="E14">
+        <v>61.404999999999994</v>
+      </c>
+      <c r="E14" s="1">
         <f t="shared" si="1"/>
-        <v>1092.702</v>
-      </c>
-      <c r="F14">
+        <v>62.730000000000004</v>
+      </c>
+      <c r="F14" s="1">
         <f t="shared" si="1"/>
-        <v>1119.7419999999997</v>
-      </c>
-      <c r="G14">
+        <v>66.22</v>
+      </c>
+      <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>1137.6759999999999</v>
-      </c>
-      <c r="H14">
+        <v>67.745000000000005</v>
+      </c>
+      <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>1158.5840000000001</v>
-      </c>
-      <c r="I14">
+        <v>67.134999999999991</v>
+      </c>
+      <c r="I14" s="1">
         <f t="shared" si="1"/>
-        <v>1171.8679999999999</v>
-      </c>
-      <c r="J14">
+        <v>67.632499999999993</v>
+      </c>
+      <c r="J14" s="1">
         <f t="shared" si="1"/>
-        <v>1181.462</v>
-      </c>
-      <c r="K14">
-        <f>SUM(K9:K13)/5</f>
-        <v>1197.5920000000001</v>
+        <v>68.452500000000001</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="1"/>
+        <v>72.294999999999987</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -13787,43 +13702,43 @@
       </c>
       <c r="B16" s="1">
         <f>B8/B14</f>
-        <v>1.5686037229111078</v>
+        <v>4.0550998025882867</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" ref="C16:K16" si="2">C8/C14</f>
-        <v>2.3813972294155592</v>
+        <f t="shared" ref="C16:J16" si="2">C8/C14</f>
+        <v>7.2561079424533919</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="2"/>
-        <v>3.1181925084824464</v>
+        <v>10.069090464945853</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="2"/>
-        <v>3.835431801168113</v>
+        <v>13.112466124661246</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="2"/>
-        <v>4.5336854382527418</v>
+        <v>15.364693446088795</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="2"/>
-        <v>5.1508988499361852</v>
+        <v>17.892353679238315</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="2"/>
-        <v>5.8751648564109296</v>
+        <v>20.825091234080581</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>6.5572675420781188</v>
+        <v>23.90389235944258</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="2"/>
-        <v>7.2171597563019372</v>
+        <v>26.127643256272595</v>
       </c>
       <c r="K16" s="1">
         <f>K8/K13</f>
-        <v>7.8012058484479061</v>
+        <v>26.99282037388242</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
@@ -14130,12 +14045,12 @@
         <v>1198.45</v>
       </c>
       <c r="T22">
-        <f>K6</f>
-        <v>9406.14</v>
+        <f>K5</f>
+        <v>1986.35</v>
       </c>
       <c r="U22">
         <f>K12</f>
-        <v>1203.2</v>
+        <v>73.599999999999994</v>
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
@@ -14194,8 +14109,8 @@
         <v>1172.1199999999999</v>
       </c>
       <c r="T23">
-        <f>K7</f>
-        <v>9397.33</v>
+        <f>K6</f>
+        <v>1988.15</v>
       </c>
       <c r="U23" t="e">
         <f>#REF!</f>
@@ -14235,7 +14150,7 @@
       <c r="A6" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>0.58630000000000004</v>
       </c>
     </row>
@@ -14243,7 +14158,7 @@
       <c r="A7" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.32100000000000001</v>
       </c>
     </row>
@@ -14251,7 +14166,7 @@
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>6.5600000000000006E-2</v>
       </c>
     </row>
@@ -14259,7 +14174,7 @@
       <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>2.7099999999999999E-2</v>
       </c>
     </row>
@@ -14267,7 +14182,7 @@
       <c r="A10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0</v>
       </c>
     </row>
@@ -14281,7 +14196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C241B48C-363D-49DC-B9A0-F3FCA400F26C}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -14434,13 +14349,13 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F12" s="5"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F13" s="5"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F14" s="5"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -14450,16 +14365,16 @@
         <f>SUM(B1:B7)</f>
         <v>100.02000000000002</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F16" s="5"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="5"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="5"/>
+      <c r="F18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualización memoria y código
</commit_message>
<xml_diff>
--- a/memoria/tablasygraficas.xlsx
+++ b/memoria/tablasygraficas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\tfg\memoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84177CC6-91FE-485A-9148-D105A62C4F0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA468D1-7586-42A0-9EC7-7651955A7132}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1485" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ÁRBOL" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="85">
   <si>
     <t>CUDA</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Semilla</t>
+  </si>
+  <si>
+    <t>Tiempos medios</t>
   </si>
 </sst>
 </file>
@@ -13316,11 +13319,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90F9EB2-862F-4F3C-8E66-7781ED8222A2}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G95" sqref="G95"/>
+      <selection pane="topRight" activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18790,87 +18793,87 @@
       <c r="A80" t="s">
         <v>14</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
         <f>SUM(B75:B79)/5</f>
         <v>27.256600000000002</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="1">
         <f t="shared" ref="C80" si="150">SUM(C75:C79)/5</f>
         <v>25.613999999999997</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="1">
         <f t="shared" ref="D80" si="151">SUM(D75:D79)/5</f>
         <v>1.0641650065367152</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="1">
         <f t="shared" ref="E80" si="152">SUM(E75:E79)/5</f>
         <v>31.922000000000004</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="1">
         <f t="shared" ref="F80" si="153">SUM(F75:F79)/5</f>
         <v>27.02</v>
       </c>
-      <c r="G80">
+      <c r="G80" s="1">
         <f t="shared" ref="G80" si="154">SUM(G75:G79)/5</f>
         <v>1.1814684436218132</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="1">
         <f t="shared" ref="H80" si="155">SUM(H75:H79)/5</f>
         <v>35.112000000000002</v>
       </c>
-      <c r="I80">
+      <c r="I80" s="1">
         <f t="shared" ref="I80" si="156">SUM(I75:I79)/5</f>
         <v>25.998000000000001</v>
       </c>
-      <c r="J80">
+      <c r="J80" s="1">
         <f t="shared" ref="J80" si="157">SUM(J75:J79)/5</f>
         <v>1.3506404854633935</v>
       </c>
-      <c r="K80">
+      <c r="K80" s="1">
         <f t="shared" ref="K80" si="158">SUM(K75:K79)/5</f>
         <v>38.17</v>
       </c>
-      <c r="L80">
+      <c r="L80" s="1">
         <f t="shared" ref="L80" si="159">SUM(L75:L79)/5</f>
         <v>26.326000000000001</v>
       </c>
-      <c r="M80">
+      <c r="M80" s="1">
         <f t="shared" ref="M80" si="160">SUM(M75:M79)/5</f>
         <v>1.4499562083100568</v>
       </c>
-      <c r="N80">
+      <c r="N80" s="1">
         <f t="shared" ref="N80" si="161">SUM(N75:N79)/5</f>
         <v>42.768000000000001</v>
       </c>
-      <c r="O80">
+      <c r="O80" s="1">
         <f t="shared" ref="O80" si="162">SUM(O75:O79)/5</f>
         <v>27.442</v>
       </c>
-      <c r="P80">
+      <c r="P80" s="1">
         <f t="shared" ref="P80" si="163">SUM(P75:P79)/5</f>
         <v>1.5585394927529836</v>
       </c>
-      <c r="Q80">
+      <c r="Q80" s="1">
         <f t="shared" ref="Q80" si="164">SUM(Q75:Q79)/5</f>
         <v>48.378</v>
       </c>
-      <c r="R80">
+      <c r="R80" s="1">
         <f t="shared" ref="R80" si="165">SUM(R75:R79)/5</f>
         <v>30.154000000000003</v>
       </c>
-      <c r="S80">
+      <c r="S80" s="1">
         <f t="shared" ref="S80" si="166">SUM(S75:S79)/5</f>
         <v>1.6043870483656879</v>
       </c>
-      <c r="T80">
+      <c r="T80" s="1">
         <f t="shared" ref="T80" si="167">SUM(T75:T79)/5</f>
         <v>48.803999999999995</v>
       </c>
-      <c r="U80">
+      <c r="U80" s="1">
         <f t="shared" ref="U80" si="168">SUM(U75:U79)/5</f>
         <v>33.613999999999997</v>
       </c>
-      <c r="V80">
+      <c r="V80" s="1">
         <f t="shared" ref="V80" si="169">SUM(V75:V79)/5</f>
         <v>1.4519321369503331</v>
       </c>
@@ -19197,6 +19200,142 @@
       <c r="H94">
         <f>SUM(H84:H93)/10</f>
         <v>79.253999999999991</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="97" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>4</v>
+      </c>
+      <c r="E97">
+        <v>5</v>
+      </c>
+      <c r="H97">
+        <v>6</v>
+      </c>
+      <c r="K97">
+        <v>7</v>
+      </c>
+      <c r="N97">
+        <v>8</v>
+      </c>
+      <c r="Q97">
+        <v>9</v>
+      </c>
+      <c r="T97">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B98" s="1">
+        <f>(B80+B72+B64+B56+B48+B40+B32+B24+B16+B8)/10</f>
+        <v>27.640120000000003</v>
+      </c>
+      <c r="C98" s="1">
+        <f>(C80+C72+C64+C56+C48+C40+C32+C24+C16+C8)/10</f>
+        <v>25.583000000000002</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1">
+        <f t="shared" ref="E98:F98" si="171">(E80+E72+E64+E56+E48+E40+E32+E24+E16+E8)/10</f>
+        <v>31.708199999999998</v>
+      </c>
+      <c r="F98" s="1">
+        <f t="shared" si="171"/>
+        <v>26.058600000000002</v>
+      </c>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1">
+        <f t="shared" ref="H98:I98" si="172">(H80+H72+H64+H56+H48+H40+H32+H24+H16+H8)/10</f>
+        <v>35.302599999999998</v>
+      </c>
+      <c r="I98" s="1">
+        <f t="shared" si="172"/>
+        <v>26.1966</v>
+      </c>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1">
+        <f t="shared" ref="K98:L98" si="173">(K80+K72+K64+K56+K48+K40+K32+K24+K16+K8)/10</f>
+        <v>38.187799999999996</v>
+      </c>
+      <c r="L98" s="1">
+        <f t="shared" si="173"/>
+        <v>26.453600000000002</v>
+      </c>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1">
+        <f t="shared" ref="N98:O98" si="174">(N80+N72+N64+N56+N48+N40+N32+N24+N16+N8)/10</f>
+        <v>40.872399999999999</v>
+      </c>
+      <c r="O98" s="1">
+        <f t="shared" si="174"/>
+        <v>27.344399999999997</v>
+      </c>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1">
+        <f t="shared" ref="Q98:R98" si="175">(Q80+Q72+Q64+Q56+Q48+Q40+Q32+Q24+Q16+Q8)/10</f>
+        <v>45.853200000000001</v>
+      </c>
+      <c r="R98" s="1">
+        <f t="shared" si="175"/>
+        <v>29.968600000000002</v>
+      </c>
+      <c r="S98" s="1"/>
+      <c r="T98" s="1">
+        <f t="shared" ref="T98:U98" si="176">(T80+T72+T64+T56+T48+T40+T32+T24+T16+T8)/10</f>
+        <v>48.662600000000005</v>
+      </c>
+      <c r="U98" s="1">
+        <f t="shared" si="176"/>
+        <v>33.629399999999997</v>
+      </c>
+    </row>
+    <row r="99" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>70</v>
+      </c>
+      <c r="C99" t="s">
+        <v>71</v>
+      </c>
+      <c r="E99" t="s">
+        <v>70</v>
+      </c>
+      <c r="F99" t="s">
+        <v>71</v>
+      </c>
+      <c r="H99" t="s">
+        <v>70</v>
+      </c>
+      <c r="I99" t="s">
+        <v>71</v>
+      </c>
+      <c r="K99" t="s">
+        <v>70</v>
+      </c>
+      <c r="L99" t="s">
+        <v>71</v>
+      </c>
+      <c r="N99" t="s">
+        <v>70</v>
+      </c>
+      <c r="O99" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>70</v>
+      </c>
+      <c r="R99" t="s">
+        <v>71</v>
+      </c>
+      <c r="T99" t="s">
+        <v>70</v>
+      </c>
+      <c r="U99" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>